<commit_message>
New documents version: 21/04/2021.
</commit_message>
<xml_diff>
--- a/documents/Questionaire COVID-19.xlsx
+++ b/documents/Questionaire COVID-19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpalbino/Downloads/COVID-19 Student Impact Study/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpalbino/Library/Mobile Documents/com~apple~CloudDocs/GitHub/covid-v1/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3104BB04-B545-EE45-82D5-FBF1C53CABF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E894976E-F896-6F4A-9074-3FF90FADE38E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35460" yWindow="1440" windowWidth="27640" windowHeight="15940" xr2:uid="{BD2B9B8F-EF0C-BE45-ABAF-38EEDD9DDC79}"/>
+    <workbookView xWindow="34920" yWindow="7720" windowWidth="27640" windowHeight="15940" xr2:uid="{BD2B9B8F-EF0C-BE45-ABAF-38EEDD9DDC79}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12411,61 +12411,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -12475,6 +12436,45 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -15627,7 +15627,7 @@
   <dimension ref="A1:D162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15638,20 +15638,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="27"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -15660,14 +15660,14 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2">
@@ -15678,8 +15678,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="2">
         <v>2</v>
       </c>
@@ -15688,8 +15688,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="2">
         <v>3</v>
       </c>
@@ -15698,9 +15698,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="20">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="13">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -15708,18 +15708,18 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2">
@@ -15730,8 +15730,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="2">
         <v>2</v>
       </c>
@@ -15740,8 +15740,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="21"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="2">
         <v>3</v>
       </c>
@@ -15750,8 +15750,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="21"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="2">
         <v>4</v>
       </c>
@@ -15760,8 +15760,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="2">
         <v>5</v>
       </c>
@@ -15770,10 +15770,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="2">
@@ -15784,8 +15784,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="2">
         <v>1</v>
       </c>
@@ -15794,10 +15794,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="2">
@@ -15808,8 +15808,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="2">
         <v>0</v>
       </c>
@@ -15818,10 +15818,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="2">
@@ -15832,8 +15832,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="2">
         <v>0</v>
       </c>
@@ -15842,30 +15842,30 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
     </row>
     <row r="22" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -15874,14 +15874,14 @@
       <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
     </row>
     <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="2">
@@ -15892,9 +15892,9 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="20">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="13">
         <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -15902,15 +15902,15 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A27" s="19"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="20">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="13">
         <v>3</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -15918,15 +15918,15 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="20">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="13">
         <v>4</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -15934,16 +15934,16 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="13" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="2">
@@ -15954,8 +15954,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="14"/>
       <c r="C32" s="2">
         <v>0</v>
       </c>
@@ -15964,10 +15964,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="2">
@@ -15978,8 +15978,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="21"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="2">
         <v>2</v>
       </c>
@@ -15988,8 +15988,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="22"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="2">
         <v>3</v>
       </c>
@@ -15998,7 +15998,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -16012,7 +16012,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="3" t="s">
         <v>46</v>
       </c>
@@ -16024,18 +16024,18 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="16"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="24"/>
     </row>
     <row r="39" spans="1:4" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C39" s="2">
@@ -16046,8 +16046,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="22"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="2">
         <v>0</v>
       </c>
@@ -16056,13 +16056,13 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="20">
+      <c r="C41" s="13">
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
@@ -16070,17 +16070,17 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="22"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="19"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="20">
+      <c r="A43" s="15"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="13">
         <v>2</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -16088,17 +16088,17 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="22"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="19"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="20">
+      <c r="A45" s="15"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="13">
         <v>3</v>
       </c>
       <c r="D45" s="3" t="s">
@@ -16106,24 +16106,24 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A46" s="19"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="22"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="14"/>
       <c r="D47" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-      <c r="B48" s="22"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="14"/>
       <c r="C48" s="2">
         <v>4</v>
       </c>
@@ -16132,7 +16132,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -16146,7 +16146,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="7" t="s">
         <v>62</v>
       </c>
@@ -16158,7 +16158,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="8"/>
       <c r="C51" s="2">
         <v>2</v>
@@ -16168,7 +16168,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="8"/>
       <c r="C52" s="2">
         <v>3</v>
@@ -16178,7 +16178,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="8"/>
       <c r="C53" s="2">
         <v>4</v>
@@ -16188,7 +16188,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
+      <c r="A54" s="12"/>
       <c r="B54" s="9"/>
       <c r="C54" s="2">
         <v>5</v>
@@ -16198,10 +16198,10 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="13" t="s">
         <v>70</v>
       </c>
       <c r="C55" s="2">
@@ -16212,8 +16212,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
-      <c r="B56" s="21"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="16"/>
       <c r="C56" s="2">
         <v>1</v>
       </c>
@@ -16222,8 +16222,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
-      <c r="B57" s="21"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="16"/>
       <c r="C57" s="2">
         <v>2</v>
       </c>
@@ -16232,8 +16232,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
-      <c r="B58" s="21"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="16"/>
       <c r="C58" s="2">
         <v>3</v>
       </c>
@@ -16242,8 +16242,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="21"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="16"/>
       <c r="C59" s="2">
         <v>4</v>
       </c>
@@ -16252,8 +16252,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
-      <c r="B60" s="22"/>
+      <c r="A60" s="12"/>
+      <c r="B60" s="14"/>
       <c r="C60" s="2">
         <v>5</v>
       </c>
@@ -16262,10 +16262,10 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C61" s="2">
@@ -16276,8 +16276,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="19"/>
-      <c r="B62" s="21"/>
+      <c r="A62" s="15"/>
+      <c r="B62" s="16"/>
       <c r="C62" s="2">
         <v>1</v>
       </c>
@@ -16286,8 +16286,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
-      <c r="B63" s="21"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
       <c r="C63" s="2">
         <v>2</v>
       </c>
@@ -16296,8 +16296,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="19"/>
-      <c r="B64" s="21"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="16"/>
       <c r="C64" s="2">
         <v>3</v>
       </c>
@@ -16306,8 +16306,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="19"/>
-      <c r="B65" s="21"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="16"/>
       <c r="C65" s="2">
         <v>4</v>
       </c>
@@ -16316,8 +16316,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
-      <c r="B66" s="22"/>
+      <c r="A66" s="12"/>
+      <c r="B66" s="14"/>
       <c r="C66" s="2">
         <v>5</v>
       </c>
@@ -16326,10 +16326,10 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="13" t="s">
         <v>74</v>
       </c>
       <c r="C67" s="2">
@@ -16340,8 +16340,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
-      <c r="B68" s="21"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="16"/>
       <c r="C68" s="2">
         <v>1</v>
       </c>
@@ -16350,8 +16350,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
-      <c r="B69" s="21"/>
+      <c r="A69" s="15"/>
+      <c r="B69" s="16"/>
       <c r="C69" s="2">
         <v>2</v>
       </c>
@@ -16360,8 +16360,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
-      <c r="B70" s="21"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="16"/>
       <c r="C70" s="2">
         <v>3</v>
       </c>
@@ -16370,8 +16370,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="19"/>
-      <c r="B71" s="21"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="16"/>
       <c r="C71" s="2">
         <v>4</v>
       </c>
@@ -16380,8 +16380,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="18"/>
-      <c r="B72" s="22"/>
+      <c r="A72" s="12"/>
+      <c r="B72" s="14"/>
       <c r="C72" s="2">
         <v>5</v>
       </c>
@@ -16390,10 +16390,10 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
+      <c r="A73" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C73" s="2">
@@ -16404,8 +16404,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="19"/>
-      <c r="B74" s="21"/>
+      <c r="A74" s="15"/>
+      <c r="B74" s="16"/>
       <c r="C74" s="2">
         <v>1</v>
       </c>
@@ -16414,8 +16414,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="29"/>
-      <c r="B75" s="29"/>
+      <c r="A75" s="31"/>
+      <c r="B75" s="31"/>
       <c r="C75" s="2">
         <v>2</v>
       </c>
@@ -16424,8 +16424,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
-      <c r="B76" s="29"/>
+      <c r="A76" s="31"/>
+      <c r="B76" s="31"/>
       <c r="C76" s="2">
         <v>3</v>
       </c>
@@ -16434,8 +16434,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
-      <c r="B77" s="29"/>
+      <c r="A77" s="31"/>
+      <c r="B77" s="31"/>
       <c r="C77" s="2">
         <v>4</v>
       </c>
@@ -16444,8 +16444,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="28"/>
-      <c r="B78" s="28"/>
+      <c r="A78" s="32"/>
+      <c r="B78" s="32"/>
       <c r="C78" s="2">
         <v>5</v>
       </c>
@@ -16454,10 +16454,10 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B79" s="20" t="s">
+      <c r="B79" s="13" t="s">
         <v>78</v>
       </c>
       <c r="C79" s="2">
@@ -16468,8 +16468,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="19"/>
-      <c r="B80" s="21"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="16"/>
       <c r="C80" s="2">
         <v>1</v>
       </c>
@@ -16478,8 +16478,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="19"/>
-      <c r="B81" s="21"/>
+      <c r="A81" s="15"/>
+      <c r="B81" s="16"/>
       <c r="C81" s="2">
         <v>2</v>
       </c>
@@ -16488,8 +16488,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="19"/>
-      <c r="B82" s="21"/>
+      <c r="A82" s="15"/>
+      <c r="B82" s="16"/>
       <c r="C82" s="2">
         <v>3</v>
       </c>
@@ -16498,8 +16498,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="19"/>
-      <c r="B83" s="21"/>
+      <c r="A83" s="15"/>
+      <c r="B83" s="16"/>
       <c r="C83" s="2">
         <v>4</v>
       </c>
@@ -16508,8 +16508,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="18"/>
-      <c r="B84" s="22"/>
+      <c r="A84" s="12"/>
+      <c r="B84" s="14"/>
       <c r="C84" s="2">
         <v>5</v>
       </c>
@@ -16524,11 +16524,11 @@
       <c r="B85" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C85" s="11"/>
-      <c r="D85" s="12"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="26"/>
     </row>
     <row r="86" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="17" t="s">
+      <c r="A86" s="11" t="s">
         <v>80</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -16542,7 +16542,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="19"/>
+      <c r="A87" s="15"/>
       <c r="B87" s="7" t="s">
         <v>62</v>
       </c>
@@ -16554,7 +16554,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="18"/>
+      <c r="A88" s="12"/>
       <c r="B88" s="9"/>
       <c r="C88" s="2">
         <v>3</v>
@@ -16564,10 +16564,10 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
+      <c r="A89" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="20" t="s">
+      <c r="B89" s="13" t="s">
         <v>86</v>
       </c>
       <c r="C89" s="2">
@@ -16578,8 +16578,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="19"/>
-      <c r="B90" s="21"/>
+      <c r="A90" s="15"/>
+      <c r="B90" s="16"/>
       <c r="C90" s="2">
         <v>2</v>
       </c>
@@ -16588,8 +16588,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="18"/>
-      <c r="B91" s="22"/>
+      <c r="A91" s="12"/>
+      <c r="B91" s="14"/>
       <c r="C91" s="2">
         <v>3</v>
       </c>
@@ -16598,10 +16598,10 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="17" t="s">
+      <c r="A92" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B92" s="20" t="s">
+      <c r="B92" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C92" s="2">
@@ -16612,8 +16612,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="19"/>
-      <c r="B93" s="21"/>
+      <c r="A93" s="15"/>
+      <c r="B93" s="16"/>
       <c r="C93" s="2">
         <v>2</v>
       </c>
@@ -16622,8 +16622,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="18"/>
-      <c r="B94" s="22"/>
+      <c r="A94" s="12"/>
+      <c r="B94" s="14"/>
       <c r="C94" s="2">
         <v>3</v>
       </c>
@@ -16632,10 +16632,10 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
+      <c r="A95" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B95" s="20" t="s">
+      <c r="B95" s="13" t="s">
         <v>90</v>
       </c>
       <c r="C95" s="2">
@@ -16646,8 +16646,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="19"/>
-      <c r="B96" s="21"/>
+      <c r="A96" s="15"/>
+      <c r="B96" s="16"/>
       <c r="C96" s="2">
         <v>2</v>
       </c>
@@ -16656,8 +16656,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="18"/>
-      <c r="B97" s="22"/>
+      <c r="A97" s="12"/>
+      <c r="B97" s="14"/>
       <c r="C97" s="2">
         <v>3</v>
       </c>
@@ -16666,10 +16666,10 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
+      <c r="A98" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B98" s="20" t="s">
+      <c r="B98" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C98" s="2">
@@ -16680,8 +16680,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="19"/>
-      <c r="B99" s="21"/>
+      <c r="A99" s="15"/>
+      <c r="B99" s="16"/>
       <c r="C99" s="2">
         <v>2</v>
       </c>
@@ -16690,8 +16690,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="18"/>
-      <c r="B100" s="22"/>
+      <c r="A100" s="12"/>
+      <c r="B100" s="14"/>
       <c r="C100" s="2">
         <v>3</v>
       </c>
@@ -16700,10 +16700,10 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="17" t="s">
+      <c r="A101" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B101" s="20" t="s">
+      <c r="B101" s="13" t="s">
         <v>94</v>
       </c>
       <c r="C101" s="2">
@@ -16714,8 +16714,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="19"/>
-      <c r="B102" s="21"/>
+      <c r="A102" s="15"/>
+      <c r="B102" s="16"/>
       <c r="C102" s="2">
         <v>2</v>
       </c>
@@ -16724,8 +16724,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="19"/>
-      <c r="B103" s="21"/>
+      <c r="A103" s="15"/>
+      <c r="B103" s="16"/>
       <c r="C103" s="2">
         <v>3</v>
       </c>
@@ -16734,8 +16734,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="19"/>
-      <c r="B104" s="21"/>
+      <c r="A104" s="15"/>
+      <c r="B104" s="16"/>
       <c r="C104" s="2">
         <v>4</v>
       </c>
@@ -16744,8 +16744,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="18"/>
-      <c r="B105" s="22"/>
+      <c r="A105" s="12"/>
+      <c r="B105" s="14"/>
       <c r="C105" s="2">
         <v>5</v>
       </c>
@@ -16754,177 +16754,177 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="17" t="s">
+      <c r="A106" s="11" t="s">
         <v>99</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C106" s="11"/>
-      <c r="D106" s="12"/>
+      <c r="C106" s="25"/>
+      <c r="D106" s="26"/>
     </row>
     <row r="107" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="18"/>
+      <c r="A107" s="12"/>
       <c r="B107" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C107" s="13"/>
-      <c r="D107" s="14"/>
+      <c r="C107" s="29"/>
+      <c r="D107" s="30"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="17" t="s">
+      <c r="A108" s="11" t="s">
         <v>102</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C108" s="11"/>
-      <c r="D108" s="12"/>
+      <c r="C108" s="25"/>
+      <c r="D108" s="26"/>
     </row>
     <row r="109" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="18"/>
+      <c r="A109" s="12"/>
       <c r="B109" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C109" s="13"/>
-      <c r="D109" s="14"/>
+      <c r="C109" s="29"/>
+      <c r="D109" s="30"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="17" t="s">
+      <c r="A110" s="11" t="s">
         <v>104</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C110" s="11"/>
-      <c r="D110" s="12"/>
+      <c r="C110" s="25"/>
+      <c r="D110" s="26"/>
     </row>
     <row r="111" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="18"/>
+      <c r="A111" s="12"/>
       <c r="B111" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C111" s="13"/>
-      <c r="D111" s="14"/>
+      <c r="C111" s="29"/>
+      <c r="D111" s="30"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" s="17" t="s">
+      <c r="A112" s="11" t="s">
         <v>106</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C112" s="11"/>
-      <c r="D112" s="12"/>
+      <c r="C112" s="25"/>
+      <c r="D112" s="26"/>
     </row>
     <row r="113" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="18"/>
+      <c r="A113" s="12"/>
       <c r="B113" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C113" s="13"/>
-      <c r="D113" s="14"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="30"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="17" t="s">
+      <c r="A114" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C114" s="11"/>
-      <c r="D114" s="12"/>
+      <c r="C114" s="25"/>
+      <c r="D114" s="26"/>
     </row>
     <row r="115" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="18"/>
+      <c r="A115" s="12"/>
       <c r="B115" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C115" s="13"/>
-      <c r="D115" s="14"/>
+      <c r="C115" s="29"/>
+      <c r="D115" s="30"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" s="17" t="s">
+      <c r="A116" s="11" t="s">
         <v>110</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C116" s="11"/>
-      <c r="D116" s="12"/>
+      <c r="C116" s="25"/>
+      <c r="D116" s="26"/>
     </row>
     <row r="117" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="18"/>
+      <c r="A117" s="12"/>
       <c r="B117" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C117" s="13"/>
-      <c r="D117" s="14"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="30"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" s="17" t="s">
+      <c r="A118" s="11" t="s">
         <v>112</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C118" s="11"/>
-      <c r="D118" s="12"/>
+      <c r="C118" s="25"/>
+      <c r="D118" s="26"/>
     </row>
     <row r="119" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="18"/>
+      <c r="A119" s="12"/>
       <c r="B119" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C119" s="13"/>
-      <c r="D119" s="14"/>
+      <c r="C119" s="29"/>
+      <c r="D119" s="30"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="17" t="s">
+      <c r="A120" s="11" t="s">
         <v>114</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C120" s="11"/>
-      <c r="D120" s="12"/>
+      <c r="C120" s="25"/>
+      <c r="D120" s="26"/>
     </row>
     <row r="121" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="18"/>
+      <c r="A121" s="12"/>
       <c r="B121" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C121" s="13"/>
-      <c r="D121" s="14"/>
+      <c r="C121" s="29"/>
+      <c r="D121" s="30"/>
     </row>
     <row r="122" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A122" s="17" t="s">
+      <c r="A122" s="11" t="s">
         <v>116</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C122" s="11"/>
-      <c r="D122" s="12"/>
+      <c r="C122" s="25"/>
+      <c r="D122" s="26"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A123" s="19"/>
+      <c r="A123" s="15"/>
       <c r="B123" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C123" s="23"/>
-      <c r="D123" s="26"/>
+      <c r="C123" s="27"/>
+      <c r="D123" s="28"/>
     </row>
     <row r="124" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="18"/>
+      <c r="A124" s="12"/>
       <c r="B124" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C124" s="13"/>
-      <c r="D124" s="14"/>
+      <c r="C124" s="29"/>
+      <c r="D124" s="30"/>
     </row>
     <row r="125" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="17" t="s">
+      <c r="A125" s="11" t="s">
         <v>118</v>
       </c>
       <c r="B125" s="3" t="s">
@@ -16938,7 +16938,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="19"/>
+      <c r="A126" s="15"/>
       <c r="B126" s="3"/>
       <c r="C126" s="2">
         <v>2</v>
@@ -16948,7 +16948,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="18"/>
+      <c r="A127" s="12"/>
       <c r="B127" s="9"/>
       <c r="C127" s="2">
         <v>3</v>
@@ -16964,8 +16964,8 @@
       <c r="B128" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C128" s="15"/>
-      <c r="D128" s="16"/>
+      <c r="C128" s="23"/>
+      <c r="D128" s="24"/>
     </row>
     <row r="129" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
@@ -16974,8 +16974,8 @@
       <c r="B129" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C129" s="15"/>
-      <c r="D129" s="15"/>
+      <c r="C129" s="23"/>
+      <c r="D129" s="23"/>
     </row>
     <row r="130" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
@@ -16984,8 +16984,8 @@
       <c r="B130" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C130" s="15"/>
-      <c r="D130" s="15"/>
+      <c r="C130" s="23"/>
+      <c r="D130" s="23"/>
     </row>
     <row r="131" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
@@ -16994,37 +16994,37 @@
       <c r="B131" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C131" s="15"/>
-      <c r="D131" s="15"/>
+      <c r="C131" s="23"/>
+      <c r="D131" s="23"/>
     </row>
     <row r="132" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A132" s="17" t="s">
+      <c r="A132" s="11" t="s">
         <v>129</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C132" s="11"/>
-      <c r="D132" s="11"/>
+      <c r="C132" s="25"/>
+      <c r="D132" s="25"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" s="19"/>
+      <c r="A133" s="15"/>
       <c r="B133" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C133" s="23"/>
-      <c r="D133" s="23"/>
+      <c r="C133" s="27"/>
+      <c r="D133" s="27"/>
     </row>
     <row r="134" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="18"/>
+      <c r="A134" s="12"/>
       <c r="B134" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C134" s="13"/>
-      <c r="D134" s="13"/>
+      <c r="C134" s="29"/>
+      <c r="D134" s="29"/>
     </row>
     <row r="135" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="17" t="s">
+      <c r="A135" s="11" t="s">
         <v>132</v>
       </c>
       <c r="B135" s="3" t="s">
@@ -17038,7 +17038,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="19"/>
+      <c r="A136" s="15"/>
       <c r="B136" s="7" t="s">
         <v>62</v>
       </c>
@@ -17050,7 +17050,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="19"/>
+      <c r="A137" s="15"/>
       <c r="B137" s="8"/>
       <c r="C137" s="2">
         <v>2</v>
@@ -17060,7 +17060,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="19"/>
+      <c r="A138" s="15"/>
       <c r="B138" s="8"/>
       <c r="C138" s="2">
         <v>3</v>
@@ -17070,7 +17070,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="19"/>
+      <c r="A139" s="15"/>
       <c r="B139" s="8"/>
       <c r="C139" s="2">
         <v>4</v>
@@ -17080,7 +17080,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="18"/>
+      <c r="A140" s="12"/>
       <c r="B140" s="9"/>
       <c r="C140" s="2">
         <v>5</v>
@@ -17090,10 +17090,10 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="17" t="s">
+      <c r="A141" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B141" s="20" t="s">
+      <c r="B141" s="13" t="s">
         <v>135</v>
       </c>
       <c r="C141" s="2">
@@ -17104,8 +17104,8 @@
       </c>
     </row>
     <row r="142" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="19"/>
-      <c r="B142" s="21"/>
+      <c r="A142" s="15"/>
+      <c r="B142" s="16"/>
       <c r="C142" s="2">
         <v>1</v>
       </c>
@@ -17114,8 +17114,8 @@
       </c>
     </row>
     <row r="143" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="19"/>
-      <c r="B143" s="21"/>
+      <c r="A143" s="15"/>
+      <c r="B143" s="16"/>
       <c r="C143" s="2">
         <v>2</v>
       </c>
@@ -17124,8 +17124,8 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="19"/>
-      <c r="B144" s="21"/>
+      <c r="A144" s="15"/>
+      <c r="B144" s="16"/>
       <c r="C144" s="2">
         <v>3</v>
       </c>
@@ -17134,8 +17134,8 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="19"/>
-      <c r="B145" s="21"/>
+      <c r="A145" s="15"/>
+      <c r="B145" s="16"/>
       <c r="C145" s="2">
         <v>4</v>
       </c>
@@ -17144,8 +17144,8 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="18"/>
-      <c r="B146" s="22"/>
+      <c r="A146" s="12"/>
+      <c r="B146" s="14"/>
       <c r="C146" s="2">
         <v>5</v>
       </c>
@@ -17154,10 +17154,10 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="17" t="s">
+      <c r="A147" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B147" s="20" t="s">
+      <c r="B147" s="13" t="s">
         <v>137</v>
       </c>
       <c r="C147" s="2">
@@ -17168,8 +17168,8 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="19"/>
-      <c r="B148" s="21"/>
+      <c r="A148" s="15"/>
+      <c r="B148" s="16"/>
       <c r="C148" s="2">
         <v>1</v>
       </c>
@@ -17178,8 +17178,8 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="19"/>
-      <c r="B149" s="21"/>
+      <c r="A149" s="15"/>
+      <c r="B149" s="16"/>
       <c r="C149" s="2">
         <v>2</v>
       </c>
@@ -17188,8 +17188,8 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="19"/>
-      <c r="B150" s="21"/>
+      <c r="A150" s="15"/>
+      <c r="B150" s="16"/>
       <c r="C150" s="2">
         <v>3</v>
       </c>
@@ -17198,8 +17198,8 @@
       </c>
     </row>
     <row r="151" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="19"/>
-      <c r="B151" s="21"/>
+      <c r="A151" s="15"/>
+      <c r="B151" s="16"/>
       <c r="C151" s="2">
         <v>4</v>
       </c>
@@ -17208,8 +17208,8 @@
       </c>
     </row>
     <row r="152" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="18"/>
-      <c r="B152" s="22"/>
+      <c r="A152" s="12"/>
+      <c r="B152" s="14"/>
       <c r="C152" s="2">
         <v>5</v>
       </c>
@@ -17218,10 +17218,10 @@
       </c>
     </row>
     <row r="153" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="17" t="s">
+      <c r="A153" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="B153" s="20" t="s">
+      <c r="B153" s="13" t="s">
         <v>139</v>
       </c>
       <c r="C153" s="2">
@@ -17232,8 +17232,8 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="19"/>
-      <c r="B154" s="21"/>
+      <c r="A154" s="15"/>
+      <c r="B154" s="16"/>
       <c r="C154" s="2">
         <v>1</v>
       </c>
@@ -17242,8 +17242,8 @@
       </c>
     </row>
     <row r="155" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="19"/>
-      <c r="B155" s="21"/>
+      <c r="A155" s="15"/>
+      <c r="B155" s="16"/>
       <c r="C155" s="2">
         <v>2</v>
       </c>
@@ -17252,8 +17252,8 @@
       </c>
     </row>
     <row r="156" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="19"/>
-      <c r="B156" s="21"/>
+      <c r="A156" s="15"/>
+      <c r="B156" s="16"/>
       <c r="C156" s="2">
         <v>3</v>
       </c>
@@ -17262,8 +17262,8 @@
       </c>
     </row>
     <row r="157" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="19"/>
-      <c r="B157" s="21"/>
+      <c r="A157" s="15"/>
+      <c r="B157" s="16"/>
       <c r="C157" s="2">
         <v>4</v>
       </c>
@@ -17272,8 +17272,8 @@
       </c>
     </row>
     <row r="158" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="18"/>
-      <c r="B158" s="22"/>
+      <c r="A158" s="12"/>
+      <c r="B158" s="14"/>
       <c r="C158" s="2">
         <v>5</v>
       </c>
@@ -17282,81 +17282,91 @@
       </c>
     </row>
     <row r="159" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A159" s="17" t="s">
+      <c r="A159" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C159" s="11"/>
-      <c r="D159" s="11"/>
+      <c r="C159" s="25"/>
+      <c r="D159" s="25"/>
     </row>
     <row r="160" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="18"/>
+      <c r="A160" s="12"/>
       <c r="B160" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C160" s="13"/>
-      <c r="D160" s="13"/>
+      <c r="C160" s="29"/>
+      <c r="D160" s="29"/>
     </row>
     <row r="161" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A161" s="17" t="s">
+      <c r="A161" s="11" t="s">
         <v>143</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C161" s="11"/>
-      <c r="D161" s="11"/>
+      <c r="C161" s="25"/>
+      <c r="D161" s="25"/>
     </row>
     <row r="162" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="18"/>
+      <c r="A162" s="12"/>
       <c r="B162" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C162" s="13"/>
-      <c r="D162" s="13"/>
+      <c r="C162" s="29"/>
+      <c r="D162" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="C20:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A41:A48"/>
-    <mergeCell ref="B41:B48"/>
-    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="C116:D117"/>
+    <mergeCell ref="C114:D115"/>
+    <mergeCell ref="C112:D113"/>
+    <mergeCell ref="C110:D111"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C122:D124"/>
+    <mergeCell ref="A141:A146"/>
+    <mergeCell ref="B141:B146"/>
+    <mergeCell ref="A135:A140"/>
+    <mergeCell ref="C120:D121"/>
+    <mergeCell ref="C118:D119"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="C132:D134"/>
+    <mergeCell ref="A122:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="C161:D162"/>
+    <mergeCell ref="A153:A158"/>
+    <mergeCell ref="B153:B158"/>
+    <mergeCell ref="A147:A152"/>
+    <mergeCell ref="B147:B152"/>
+    <mergeCell ref="A159:A160"/>
+    <mergeCell ref="C159:D160"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="A101:A105"/>
+    <mergeCell ref="B101:B105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="C106:D107"/>
+    <mergeCell ref="C108:D109"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="B98:B100"/>
     <mergeCell ref="A75:A78"/>
     <mergeCell ref="B75:B78"/>
     <mergeCell ref="A79:A84"/>
@@ -17367,54 +17377,44 @@
     <mergeCell ref="B67:B72"/>
     <mergeCell ref="A73:A74"/>
     <mergeCell ref="B73:B74"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="A101:A105"/>
-    <mergeCell ref="B101:B105"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="C106:D107"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="C108:D109"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="C161:D162"/>
-    <mergeCell ref="A153:A158"/>
-    <mergeCell ref="B153:B158"/>
-    <mergeCell ref="A147:A152"/>
-    <mergeCell ref="B147:B152"/>
-    <mergeCell ref="A141:A146"/>
-    <mergeCell ref="B141:B146"/>
-    <mergeCell ref="A135:A140"/>
-    <mergeCell ref="C120:D121"/>
-    <mergeCell ref="C118:D119"/>
-    <mergeCell ref="C116:D117"/>
-    <mergeCell ref="C114:D115"/>
-    <mergeCell ref="C112:D113"/>
-    <mergeCell ref="C110:D111"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="A159:A160"/>
-    <mergeCell ref="C159:D160"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="C132:D134"/>
-    <mergeCell ref="A122:A124"/>
-    <mergeCell ref="C122:D124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A48"/>
+    <mergeCell ref="B41:B48"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="C20:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>